<commit_message>
amelioration seeding loadings -> utilisation du controller
</commit_message>
<xml_diff>
--- a/resources/assets/excel/PalettenKonto2.xlsx
+++ b/resources/assets/excel/PalettenKonto2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="54">
   <si>
     <t>TRY1</t>
   </si>
@@ -917,10 +917,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD16"/>
+  <dimension ref="A1:AD15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AC16" sqref="AC16"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AD15" sqref="AD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <v>42777</v>
+        <v>43084</v>
       </c>
       <c r="B12" s="8">
         <v>42048</v>
@@ -2022,28 +2022,28 @@
       <c r="AC12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="AD12">
-        <v>3</v>
+      <c r="AD12" s="9">
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <v>42791</v>
+        <v>42850</v>
       </c>
       <c r="B13" s="8">
-        <v>42048</v>
+        <v>42072</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D13" s="10">
-        <v>2150011</v>
+        <v>2153486</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>6</v>
@@ -2064,10 +2064,10 @@
         <v>10</v>
       </c>
       <c r="M13" s="9">
-        <v>6421</v>
+        <v>2521</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="O13" s="9">
         <v>2</v>
@@ -2082,43 +2082,41 @@
         <v>1</v>
       </c>
       <c r="S13" s="9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="T13" s="9">
         <v>4325</v>
       </c>
       <c r="U13" s="9">
-        <v>770</v>
+        <v>860</v>
       </c>
       <c r="V13" s="9">
-        <v>700</v>
+        <v>840</v>
       </c>
       <c r="W13" s="9">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="X13" s="9">
         <v>0</v>
       </c>
       <c r="Y13" s="9" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="Z13" s="11" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="AA13" s="9"/>
-      <c r="AB13" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="AB13" s="12"/>
       <c r="AC13" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD13" s="9">
-        <v>4</v>
+        <v>19</v>
+      </c>
+      <c r="AD13" s="13">
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <v>42800</v>
+        <v>42860</v>
       </c>
       <c r="B14" s="8">
         <v>42072</v>
@@ -2190,7 +2188,7 @@
         <v>0</v>
       </c>
       <c r="Y14" s="9" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="Z14" s="11" t="s">
         <v>18</v>
@@ -2200,183 +2198,95 @@
       <c r="AC14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="AD14" s="13">
-        <v>5</v>
+      <c r="AD14" s="9">
+        <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
-        <v>42861</v>
-      </c>
-      <c r="B15" s="8">
+    <row r="15" spans="1:30" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>42741</v>
+      </c>
+      <c r="B15" s="14">
         <v>42072</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="16">
         <v>2153486</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G15" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="15">
         <v>33500</v>
       </c>
-      <c r="J15" s="9" t="s">
+      <c r="J15" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K15" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="L15" s="9" t="s">
+      <c r="L15" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="M15" s="9">
+      <c r="M15" s="15">
         <v>2521</v>
       </c>
-      <c r="N15" s="9" t="s">
+      <c r="N15" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="O15" s="9">
+      <c r="O15" s="15">
         <v>2</v>
       </c>
-      <c r="P15" s="9" t="s">
+      <c r="P15" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="Q15" s="9" t="s">
+      <c r="Q15" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="R15" s="9">
+      <c r="R15" s="15">
         <v>1</v>
       </c>
-      <c r="S15" s="9" t="s">
+      <c r="S15" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="T15" s="9">
+      <c r="T15" s="15">
         <v>4325</v>
       </c>
-      <c r="U15" s="9">
+      <c r="U15" s="15">
         <v>860</v>
       </c>
-      <c r="V15" s="9">
+      <c r="V15" s="15">
         <v>840</v>
       </c>
-      <c r="W15" s="9">
+      <c r="W15" s="15">
         <v>20</v>
       </c>
-      <c r="X15" s="9">
+      <c r="X15" s="15">
         <v>0</v>
       </c>
-      <c r="Y15" s="9" t="s">
+      <c r="Y15" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="Z15" s="11" t="s">
+      <c r="Z15" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="AA15" s="9"/>
-      <c r="AB15" s="12"/>
-      <c r="AC15" s="9" t="s">
+      <c r="AA15" s="15"/>
+      <c r="AB15" s="18"/>
+      <c r="AC15" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="AD15" s="9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>43073</v>
-      </c>
-      <c r="B16" s="8">
-        <v>42072</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="10">
-        <v>2153486</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I16" s="9">
-        <v>33500</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="L16" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="M16" s="9">
-        <v>2521</v>
-      </c>
-      <c r="N16" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="O16" s="9">
-        <v>2</v>
-      </c>
-      <c r="P16" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q16" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="R16" s="9">
-        <v>1</v>
-      </c>
-      <c r="S16" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="T16" s="9">
-        <v>4325</v>
-      </c>
-      <c r="U16" s="9">
-        <v>860</v>
-      </c>
-      <c r="V16" s="9">
-        <v>840</v>
-      </c>
-      <c r="W16" s="9">
-        <v>20</v>
-      </c>
-      <c r="X16" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z16" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA16" s="9"/>
-      <c r="AB16" s="12"/>
-      <c r="AC16" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD16">
+      <c r="AD15" s="19">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
lecture excel 1 feuille OK
</commit_message>
<xml_diff>
--- a/resources/assets/excel/PalettenKonto2.xlsx
+++ b/resources/assets/excel/PalettenKonto2.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -2296,16 +2295,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>